<commit_message>
fixes #5, fixes #6
</commit_message>
<xml_diff>
--- a/check.xlsx
+++ b/check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alant\IdeaProjects\05-TaxiService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6E0BA7A-48B7-406F-BC61-34B2995FAB7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F93D780-FBB0-42EE-A251-793A053AA409}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{0AD42B64-F271-4631-9C06-985BD8AD47A6}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>850.13699999999994</v>
+        <v>10.456</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -419,11 +419,11 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>A3+A2*A1</f>
-        <v>17062.739999999998</v>
+        <v>269.12</v>
       </c>
       <c r="B4" s="1">
         <f>A4-100</f>
-        <v>16962.739999999998</v>
+        <v>169.12</v>
       </c>
       <c r="G4">
         <f>G3*F3</f>
@@ -433,21 +433,21 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f>0.95*A4</f>
-        <v>16209.602999999997</v>
+        <v>255.66399999999999</v>
       </c>
       <c r="B5" s="2">
         <f>A5-100</f>
-        <v>16109.602999999997</v>
+        <v>155.66399999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>0.05*A4</f>
-        <v>853.13699999999994</v>
+        <v>13.456000000000001</v>
       </c>
       <c r="B6" s="1">
         <f>A4-A6</f>
-        <v>16209.602999999997</v>
+        <v>255.66400000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>